<commit_message>
added cache, fixed problem with entries, still bug
</commit_message>
<xml_diff>
--- a/resources/type_map.xlsx
+++ b/resources/type_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Documents/GitHub/processSanskrit/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F12EBD3-77AE-6B4F-8A7E-A1A2A39BDA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA97229A-CF74-6B43-ABB4-52E8E8CE67D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="394">
   <si>
     <t>abbr</t>
   </si>
@@ -1196,13 +1196,19 @@
   </si>
   <si>
     <t>perfect , middle voice</t>
+  </si>
+  <si>
+    <t>f_1_t</t>
+  </si>
+  <si>
+    <t>n_1_t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1217,6 +1223,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF495057"/>
+      <name val="Palatino"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1254,11 +1266,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1563,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B196"/>
+  <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="E182" sqref="E182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3139,6 +3152,22 @@
         <v>391</v>
       </c>
     </row>
+    <row r="197" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>393</v>
+      </c>
+      <c r="B198" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>